<commit_message>
Before Make Seperate repos
</commit_message>
<xml_diff>
--- a/DATABASE/DataSeed.xlsx
+++ b/DATABASE/DataSeed.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
+    <workbookView windowWidth="22943" windowHeight="9875" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,15 @@
     <sheet name="SqlSourceConfiguration" sheetId="6" r:id="rId6"/>
     <sheet name="GridConfiguration" sheetId="7" r:id="rId7"/>
     <sheet name="FormConfiguration" sheetId="8" r:id="rId8"/>
+    <sheet name="Tables" sheetId="9" r:id="rId9"/>
+    <sheet name="Account Types" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1607,6 +1609,9 @@
     <t>Puducherry</t>
   </si>
   <si>
+    <t>GridColumnConfiguration</t>
+  </si>
+  <si>
     <t>GridConfigId</t>
   </si>
   <si>
@@ -1706,7 +1711,247 @@
     <t>Product Category</t>
   </si>
   <si>
-    <t>GridColumnConfiguration</t>
+    <t>GrdLedgerType</t>
+  </si>
+  <si>
+    <t>TypeName</t>
+  </si>
+  <si>
+    <t>Ledger Type</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>Account Head</t>
+  </si>
+  <si>
+    <t>FormFieldConfiguration</t>
+  </si>
+  <si>
+    <t>FormConfigId</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t>CatId</t>
+  </si>
+  <si>
+    <t>MaxDate</t>
+  </si>
+  <si>
+    <t>MinDate</t>
+  </si>
+  <si>
+    <t>DisplayFormat</t>
+  </si>
+  <si>
+    <t>IsRequired</t>
+  </si>
+  <si>
+    <t>MaxValue</t>
+  </si>
+  <si>
+    <t>MinValue</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>SearchOperator</t>
+  </si>
+  <si>
+    <t>IsPrimaryKey</t>
+  </si>
+  <si>
+    <t>IsAutoGenerated</t>
+  </si>
+  <si>
+    <t>IsUpdatable</t>
+  </si>
+  <si>
+    <t>ObjectId</t>
+  </si>
+  <si>
+    <t>CatCity</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>0x0000000000009483</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>0x0000000000009484</t>
+  </si>
+  <si>
+    <t>stateId</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>datacombo</t>
+  </si>
+  <si>
+    <t>CatState</t>
+  </si>
+  <si>
+    <t>0x0000000000009485</t>
+  </si>
+  <si>
+    <t>CatCitySearch</t>
+  </si>
+  <si>
+    <t>0x000000000000948F</t>
+  </si>
+  <si>
+    <t>0x0000000000009490</t>
+  </si>
+  <si>
+    <t>CatCountry</t>
+  </si>
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>0x0000000000009480</t>
+  </si>
+  <si>
+    <t>0x000000000000947F</t>
+  </si>
+  <si>
+    <t>CatCountrySearch</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>0x000000000000948C</t>
+  </si>
+  <si>
+    <t>Like</t>
+  </si>
+  <si>
+    <t>0x000000000000948B</t>
+  </si>
+  <si>
+    <t>CatCurrency</t>
+  </si>
+  <si>
+    <t>Currency Code</t>
+  </si>
+  <si>
+    <t>0x0000000000009482</t>
+  </si>
+  <si>
+    <t>0x0000000000009481</t>
+  </si>
+  <si>
+    <t>CatCurrencySearch</t>
+  </si>
+  <si>
+    <t>0x000000000000948E</t>
+  </si>
+  <si>
+    <t>0x000000000000948D</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>0x0000000000009488</t>
+  </si>
+  <si>
+    <t>0x0000000000009486</t>
+  </si>
+  <si>
+    <t>0x0000000000009487</t>
+  </si>
+  <si>
+    <t>CatStateSearch</t>
+  </si>
+  <si>
+    <t>0x000000000000948A</t>
+  </si>
+  <si>
+    <t>0x0000000000009489</t>
+  </si>
+  <si>
+    <t>ProductCategory</t>
+  </si>
+  <si>
+    <t>0x0000000000009492</t>
+  </si>
+  <si>
+    <t>isInventory</t>
+  </si>
+  <si>
+    <t>checkbox</t>
+  </si>
+  <si>
+    <t>0x0000000000009493</t>
+  </si>
+  <si>
+    <t>0x0000000000009491</t>
+  </si>
+  <si>
+    <t>CatalogDictionary</t>
+  </si>
+  <si>
+    <t>CatalogId</t>
+  </si>
+  <si>
+    <t>TableName</t>
+  </si>
+  <si>
+    <t>DisplayColumn</t>
+  </si>
+  <si>
+    <t>ValueColumn</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>0x000000000000947D</t>
+  </si>
+  <si>
+    <t>0x000000000000947A</t>
+  </si>
+  <si>
+    <t>0x000000000000947B</t>
+  </si>
+  <si>
+    <t>0x000000000000947C</t>
+  </si>
+  <si>
+    <t>0x000000000000947E</t>
+  </si>
+  <si>
+    <t>SqlSourceConfiguration</t>
   </si>
   <si>
     <t>SqlQuery</t>
@@ -1715,9 +1960,6 @@
     <t>SqlSourceType</t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t xml:space="preserve">select C.Id, C.Name, StateId, S.Name [StateName]  From CatCity C inner join CatState S on C.StateId = S.Id </t>
   </si>
   <si>
@@ -1727,7 +1969,7 @@
     <t xml:space="preserve">select Name,Id,IsInventory From ProductCategory </t>
   </si>
   <si>
-    <t>SqlSourceConfiguration</t>
+    <t>GridConfiguration</t>
   </si>
   <si>
     <t>PageSize</t>
@@ -1745,229 +1987,37 @@
     <t>Params</t>
   </si>
   <si>
-    <t>TableName</t>
-  </si>
-  <si>
     <t>ColumnList</t>
   </si>
   <si>
-    <t>CatCitySearch</t>
-  </si>
-  <si>
     <t>/DynamicGrid/GrdCatCity</t>
   </si>
   <si>
     <t>post</t>
   </si>
   <si>
-    <t>CatCity</t>
-  </si>
-  <si>
     <t>Name,Country</t>
   </si>
   <si>
-    <t>CatCountrySearch</t>
-  </si>
-  <si>
     <t>/DynamicGrid/GrdCatCountry</t>
   </si>
   <si>
-    <t>CatCountry</t>
-  </si>
-  <si>
     <t>Name,Code</t>
   </si>
   <si>
-    <t>CatCurrencySearch</t>
-  </si>
-  <si>
     <t>/DynamicGrid/GrdCatCurrency</t>
   </si>
   <si>
-    <t>CatCurrency</t>
-  </si>
-  <si>
-    <t>CatStateSearch</t>
-  </si>
-  <si>
     <t>/DynamicGrid/GrdCatState</t>
   </si>
   <si>
-    <t>CatState</t>
-  </si>
-  <si>
     <t>/DynamicGrid/ProductCategory</t>
   </si>
   <si>
-    <t>ProductCategory</t>
-  </si>
-  <si>
     <t>Name,Id,IsInventory</t>
   </si>
   <si>
-    <t>GridConfiguration</t>
-  </si>
-  <si>
-    <t>FormFieldConfiguration</t>
-  </si>
-  <si>
-    <t>FormConfigId</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Placeholder</t>
-  </si>
-  <si>
-    <t>CatId</t>
-  </si>
-  <si>
-    <t>MaxDate</t>
-  </si>
-  <si>
-    <t>MinDate</t>
-  </si>
-  <si>
-    <t>DisplayFormat</t>
-  </si>
-  <si>
-    <t>IsRequired</t>
-  </si>
-  <si>
-    <t>MaxValue</t>
-  </si>
-  <si>
-    <t>MinValue</t>
-  </si>
-  <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>SearchOperator</t>
-  </si>
-  <si>
-    <t>IsPrimaryKey</t>
-  </si>
-  <si>
-    <t>IsAutoGenerated</t>
-  </si>
-  <si>
-    <t>IsUpdatable</t>
-  </si>
-  <si>
-    <t>ObjectId</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>hidden</t>
-  </si>
-  <si>
-    <t>0x0000000000009483</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>0x0000000000009484</t>
-  </si>
-  <si>
-    <t>stateId</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>datacombo</t>
-  </si>
-  <si>
-    <t>0x0000000000009485</t>
-  </si>
-  <si>
-    <t>0x000000000000948F</t>
-  </si>
-  <si>
-    <t>0x0000000000009490</t>
-  </si>
-  <si>
-    <t>Country Code</t>
-  </si>
-  <si>
-    <t>0x0000000000009480</t>
-  </si>
-  <si>
-    <t>0x000000000000947F</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>0x000000000000948C</t>
-  </si>
-  <si>
-    <t>Like</t>
-  </si>
-  <si>
-    <t>0x000000000000948B</t>
-  </si>
-  <si>
-    <t>Currency Code</t>
-  </si>
-  <si>
-    <t>0x0000000000009482</t>
-  </si>
-  <si>
-    <t>0x0000000000009481</t>
-  </si>
-  <si>
-    <t>0x000000000000948E</t>
-  </si>
-  <si>
-    <t>0x000000000000948D</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>0x0000000000009488</t>
-  </si>
-  <si>
-    <t>0x0000000000009486</t>
-  </si>
-  <si>
-    <t>0x0000000000009487</t>
-  </si>
-  <si>
-    <t>0x000000000000948A</t>
-  </si>
-  <si>
-    <t>0x0000000000009489</t>
-  </si>
-  <si>
-    <t>0x0000000000009492</t>
-  </si>
-  <si>
-    <t>isInventory</t>
-  </si>
-  <si>
-    <t>checkbox</t>
-  </si>
-  <si>
-    <t>0x0000000000009493</t>
-  </si>
-  <si>
-    <t>0x0000000000009491</t>
+    <t>FormConfiguration</t>
   </si>
   <si>
     <t>FormName</t>
@@ -2021,76 +2071,505 @@
     <t>55A43B6F-57F7-49E6-A199-2217E0E985CC</t>
   </si>
   <si>
-    <t>FormConfiguration</t>
-  </si>
-  <si>
-    <t>CatalogId</t>
-  </si>
-  <si>
-    <t>DisplayColumn</t>
-  </si>
-  <si>
-    <t>ValueColumn</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>0x000000000000947D</t>
-  </si>
-  <si>
-    <t>0x000000000000947A</t>
-  </si>
-  <si>
-    <t>0x000000000000947B</t>
-  </si>
-  <si>
-    <t>0x000000000000947C</t>
-  </si>
-  <si>
-    <t>0x000000000000947E</t>
-  </si>
-  <si>
-    <t>CatalogDictionary</t>
-  </si>
-  <si>
-    <t>TypeName</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>GrdLedgerType</t>
-  </si>
-  <si>
-    <t>Ledger Type</t>
-  </si>
-  <si>
-    <t>Account Head</t>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank Name </t>
+  </si>
+  <si>
+    <t>Bank Branch</t>
+  </si>
+  <si>
+    <t>IFSC Code</t>
+  </si>
+  <si>
+    <t>ACNumber</t>
+  </si>
+  <si>
+    <t>LedgerId</t>
+  </si>
+  <si>
+    <t>AC_TYPE_NAME</t>
+  </si>
+  <si>
+    <t>PARENT_TYPE</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Capital Accounts</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Cash Accounts</t>
+  </si>
+  <si>
+    <t>Current Assets</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Current Liabilities</t>
+  </si>
+  <si>
+    <t>Direct Expenses</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Direct Incomes</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Duties and Taxes</t>
+  </si>
+  <si>
+    <t>Fixed Assets</t>
+  </si>
+  <si>
+    <t>Indirect Expenses</t>
+  </si>
+  <si>
+    <t>Indirect Incomes</t>
+  </si>
+  <si>
+    <t>Investments</t>
+  </si>
+  <si>
+    <t>Loan and Advances</t>
+  </si>
+  <si>
+    <t>Loans (Liability)</t>
+  </si>
+  <si>
+    <t>Misc. Expenses (Asset)</t>
+  </si>
+  <si>
+    <t>Provisions</t>
+  </si>
+  <si>
+    <t>Purchase Accounts</t>
+  </si>
+  <si>
+    <t>Reserves and Surplus</t>
+  </si>
+  <si>
+    <t>Sales Accounts</t>
+  </si>
+  <si>
+    <t>Secured Loans</t>
+  </si>
+  <si>
+    <t>Stock on hand</t>
+  </si>
+  <si>
+    <t>Sundry Creditors</t>
+  </si>
+  <si>
+    <t>Sundry Debtors</t>
+  </si>
+  <si>
+    <t>Unsecured Loans</t>
+  </si>
+  <si>
+    <t>Pre-operative Expenses (Asset)</t>
+  </si>
+  <si>
+    <t>Securities and Deposites (Asset)</t>
+  </si>
+  <si>
+    <t>Bank Accounts</t>
+  </si>
+  <si>
+    <t>BRANCH/DIVISION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2098,18 +2577,313 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2392,19 +3166,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B246"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B246"/>
+      <selection activeCell="A1" sqref="A1:B246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4375,19 +5149,274 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="29.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="13.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>691</v>
+      </c>
+      <c r="B2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>693</v>
+      </c>
+      <c r="B3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>695</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>696</v>
+      </c>
+      <c r="B5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>698</v>
+      </c>
+      <c r="B6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>699</v>
+      </c>
+      <c r="B7" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>701</v>
+      </c>
+      <c r="B8" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>703</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>704</v>
+      </c>
+      <c r="B10" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>705</v>
+      </c>
+      <c r="B11" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>706</v>
+      </c>
+      <c r="B12" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>707</v>
+      </c>
+      <c r="B13" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>708</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>709</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>710</v>
+      </c>
+      <c r="B16" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>711</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>712</v>
+      </c>
+      <c r="B18" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>713</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>714</v>
+      </c>
+      <c r="B20" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>715</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>716</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>717</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>718</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>719</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>720</v>
+      </c>
+      <c r="B26" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>721</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>722</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>723</v>
+      </c>
+      <c r="B29">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4678,721 +5707,725 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="216.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="18.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="9.28703703703704" customWidth="1"/>
+    <col min="4" max="4" width="16.287037037037" customWidth="1"/>
+    <col min="5" max="5" width="9.85185185185185" customWidth="1"/>
+    <col min="6" max="6" width="8.13888888888889" customWidth="1"/>
+    <col min="7" max="7" width="12.712962962963" customWidth="1"/>
+    <col min="8" max="8" width="8.28703703703704" customWidth="1"/>
+    <col min="9" max="9" width="8.42592592592593" customWidth="1"/>
+    <col min="10" max="10" width="9.71296296296296" customWidth="1"/>
+    <col min="11" max="11" width="6.42592592592593" customWidth="1"/>
+    <col min="12" max="12" width="5.57407407407407" customWidth="1"/>
+    <col min="13" max="13" width="216.574074074074" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="I2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="J2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="K2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="L2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C3" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D3" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F3">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L3" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M3" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A3,"','",B3,"','",C3,"','",D3,"',",E3,",",F3,",'",G3,"',",H3,",",I3,",'",J3,"',",K3,",'",L3,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A3,"','",B3,"','",C3,"','",D3,"',",E3,",",F3,",'",G3,"',",H3,",",I3,",'",J3,"',",K3,",'",L3,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatCity','name','string','City Name',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B4" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D4" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F4">
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L4" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M4" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A4,"','",B4,"','",C4,"','",D4,"',",E4,",",F4,",'",G4,"',",H4,",",I4,",'",J4,"',",K4,",'",L4,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A4,"','",B4,"','",C4,"','",D4,"',",E4,",",F4,",'",G4,"',",H4,",",I4,",'",J4,"',",K4,",'",L4,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatCity','stateName','string','State Name',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B5" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C5" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F5">
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L5" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M5" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A5,"','",B5,"','",C5,"','",D5,"',",E5,",",F5,",'",G5,"',",H5,",",I5,",'",J5,"',",K5,",'",L5,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A5,"','",B5,"','",C5,"','",D5,"',",E5,",",F5,",'",G5,"',",H5,",",I5,",'",J5,"',",K5,",'",L5,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatCountry','code','string','Code',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B6" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D6" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M6" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A6,"','",B6,"','",C6,"','",D6,"',",E6,",",F6,",'",G6,"',",H6,",",I6,",'",J6,"',",K6,",'",L6,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A6,"','",B6,"','",C6,"','",D6,"',",E6,",",F6,",'",G6,"',",H6,",",I6,",'",J6,"',",K6,",'",L6,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatCountry','name','string','Country Name',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B7" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C7" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D7" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K7">
         <v>100</v>
       </c>
       <c r="L7" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M7" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A7,"','",B7,"','",C7,"','",D7,"',",E7,",",F7,",'",G7,"',",H7,",",I7,",'",J7,"',",K7,",'",L7,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A7,"','",B7,"','",C7,"','",D7,"',",E7,",",F7,",'",G7,"',",H7,",",I7,",'",J7,"',",K7,",'",L7,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatCurrency','code','string','Code',NULL,6,'',NULL,1,'Asc',100,'left')</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C8" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D8" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K8">
         <v>150</v>
       </c>
       <c r="L8" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M8" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A8,"','",B8,"','",C8,"','",D8,"',",E8,",",F8,",'",G8,"',",H8,",",I8,",'",J8,"',",K8,",'",L8,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A8,"','",B8,"','",C8,"','",D8,"',",E8,",",F8,",'",G8,"',",H8,",",I8,",'",J8,"',",K8,",'",L8,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatCurrency','name','string','Currency Name',NULL,6,'',NULL,1,'Asc',150,'left')</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B9" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C9" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D9" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L9" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M9" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A9,"','",B9,"','",C9,"','",D9,"',",E9,",",F9,",'",G9,"',",H9,",",I9,",'",J9,"',",K9,",'",L9,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A9,"','",B9,"','",C9,"','",D9,"',",E9,",",F9,",'",G9,"',",H9,",",I9,",'",J9,"',",K9,",'",L9,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatState','countryName','string','Country Name',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B10" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C10" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D10" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F10">
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L10" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M10" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A10,"','",B10,"','",C10,"','",D10,"',",E10,",",F10,",'",G10,"',",H10,",",I10,",'",J10,"',",K10,",'",L10,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A10,"','",B10,"','",C10,"','",D10,"',",E10,",",F10,",'",G10,"',",H10,",",I10,",'",J10,"',",K10,",'",L10,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdCatState','name','string','State Name',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B11" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C11" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D11" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F11">
         <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L11" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M11" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A11,"','",B11,"','",C11,"','",D11,"',",E11,",",F11,",'",G11,"',",H11,",",I11,",'",J11,"',",K11,",'",L11,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A11,"','",B11,"','",C11,"','",D11,"',",E11,",",F11,",'",G11,"',",H11,",",I11,",'",J11,"',",K11,",'",L11,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdProductCategory','Maintain Inventory','boolean','Currency Name',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B12" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C12" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D12" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F12">
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L12" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M12" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A12,"','",B12,"','",C12,"','",D12,"',",E12,",",F12,",'",G12,"',",H12,",",I12,",'",J12,"',",K12,",'",L12,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A12,"','",B12,"','",C12,"','",D12,"',",E12,",",F12,",'",G12,"',",H12,",",I12,",'",J12,"',",K12,",'",L12,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdProductCategory','name','string','Product Category',NULL,6,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>679</v>
+        <v>562</v>
       </c>
       <c r="B13" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C13" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D13" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F13">
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L13" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M13" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A13,"','",B13,"','",C13,"','",D13,"',",E13,",",F13,",'",G13,"',",H13,",",I13,",'",J13,"',",K13,",'",L13,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A13,"','",B13,"','",C13,"','",D13,"',",E13,",",F13,",'",G13,"',",H13,",",I13,",'",J13,"',",K13,",'",L13,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdLedgerType','Code','string','Code',NULL,4,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>679</v>
+        <v>562</v>
       </c>
       <c r="B14" t="s">
-        <v>677</v>
+        <v>563</v>
       </c>
       <c r="C14" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D14" t="s">
-        <v>680</v>
+        <v>564</v>
       </c>
       <c r="E14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F14">
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L14" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M14" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A14,"','",B14,"','",C14,"','",D14,"',",E14,",",F14,",'",G14,"',",H14,",",I14,",'",J14,"',",K14,",'",L14,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A14,"','",B14,"','",C14,"','",D14,"',",E14,",",F14,",'",G14,"',",H14,",",I14,",'",J14,"',",K14,",'",L14,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdLedgerType','TypeName','string','Ledger Type',NULL,4,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>679</v>
+        <v>562</v>
       </c>
       <c r="B15" t="s">
-        <v>678</v>
+        <v>565</v>
       </c>
       <c r="C15" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D15" t="s">
-        <v>681</v>
+        <v>566</v>
       </c>
       <c r="E15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L15" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M15" t="str">
-        <f>CONCATENATE("Insert into ",$A$1," ( ", $A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A15,"','",B15,"','",C15,"','",D15,"',",E15,",",F15,",'",G15,"',",H15,",",I15,",'",J15,"',",K15,",'",L15,"')")</f>
+        <f>CONCATENATE("Insert into ",$A$1," ( ",$A$2,",",$B$2,",",$C$2,",",$D$2,",",$E$2,",",$F$2,",",$G$2,",",$H$2,",",$I$2,",",$J$2,",",$K$2,",",$L$2," ) Values ('",A15,"','",B15,"','",C15,"','",D15,"',",E15,",",F15,",'",G15,"',",H15,",",I15,",'",J15,"',",K15,",'",L15,"')")</f>
         <v>Insert into GridColumnConfiguration ( GridConfigId,DataField,DataType,Header,Formatter,ColSpan,DefaultValue,CssClass,Sortable,SortOrder,Width,Align ) Values ('GrdLedgerType','AccountType','string','Account Head',NULL,4,'',NULL,1,'Asc',NULL,'left')</v>
       </c>
     </row>
     <row r="19" ht="26.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5740740740741" customWidth="1"/>
+    <col min="2" max="2" width="15.8518518518519" customWidth="1"/>
+    <col min="3" max="3" width="18.1388888888889" customWidth="1"/>
+    <col min="4" max="4" width="16.287037037037" customWidth="1"/>
+    <col min="5" max="5" width="39.712962962963" customWidth="1"/>
+    <col min="6" max="6" width="19.287037037037" customWidth="1"/>
+    <col min="7" max="7" width="8.85185185185185" customWidth="1"/>
+    <col min="8" max="8" width="8.57407407407407" customWidth="1"/>
+    <col min="9" max="9" width="13.8518518518519" customWidth="1"/>
+    <col min="10" max="10" width="10.5740740740741" customWidth="1"/>
+    <col min="11" max="11" width="9.85185185185185" customWidth="1"/>
+    <col min="12" max="12" width="9.57407407407407" customWidth="1"/>
+    <col min="13" max="13" width="7.57407407407407" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="12.5740740740741" customWidth="1"/>
+    <col min="16" max="16" width="16.287037037037" customWidth="1"/>
+    <col min="17" max="17" width="11.5740740740741" customWidth="1"/>
+    <col min="18" max="18" width="19.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>595</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>596</v>
+        <v>568</v>
       </c>
       <c r="B2" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="C2" t="s">
-        <v>598</v>
+        <v>570</v>
       </c>
       <c r="D2" t="s">
-        <v>599</v>
+        <v>571</v>
       </c>
       <c r="E2" t="s">
-        <v>600</v>
+        <v>572</v>
       </c>
       <c r="F2" t="s">
-        <v>601</v>
+        <v>573</v>
       </c>
       <c r="G2" t="s">
-        <v>602</v>
+        <v>574</v>
       </c>
       <c r="H2" t="s">
-        <v>603</v>
+        <v>575</v>
       </c>
       <c r="I2" t="s">
-        <v>604</v>
+        <v>576</v>
       </c>
       <c r="J2" t="s">
-        <v>605</v>
+        <v>577</v>
       </c>
       <c r="K2" t="s">
-        <v>606</v>
+        <v>578</v>
       </c>
       <c r="L2" t="s">
-        <v>607</v>
+        <v>579</v>
       </c>
       <c r="M2" t="s">
-        <v>608</v>
+        <v>580</v>
       </c>
       <c r="N2" t="s">
-        <v>609</v>
+        <v>581</v>
       </c>
       <c r="O2" t="s">
-        <v>610</v>
+        <v>582</v>
       </c>
       <c r="P2" t="s">
-        <v>611</v>
+        <v>583</v>
       </c>
       <c r="Q2" t="s">
-        <v>612</v>
+        <v>584</v>
       </c>
       <c r="R2" t="s">
-        <v>613</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="B3" t="s">
-        <v>614</v>
+        <v>587</v>
       </c>
       <c r="D3" t="s">
-        <v>615</v>
+        <v>588</v>
       </c>
       <c r="E3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -5404,51 +6437,51 @@
         <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>616</v>
+        <v>589</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="B4" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C4" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D4" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -5460,51 +6493,51 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>618</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="B5" t="s">
-        <v>619</v>
+        <v>592</v>
       </c>
       <c r="C5" t="s">
-        <v>620</v>
+        <v>593</v>
       </c>
       <c r="D5" t="s">
-        <v>621</v>
+        <v>594</v>
       </c>
       <c r="E5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F5" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="G5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -5516,51 +6549,51 @@
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>622</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>576</v>
+        <v>597</v>
       </c>
       <c r="B6" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C6" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D6" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -5572,51 +6605,51 @@
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>623</v>
+        <v>598</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>576</v>
+        <v>597</v>
       </c>
       <c r="B7" t="s">
-        <v>619</v>
+        <v>592</v>
       </c>
       <c r="C7" t="s">
-        <v>620</v>
+        <v>593</v>
       </c>
       <c r="D7" t="s">
-        <v>621</v>
+        <v>594</v>
       </c>
       <c r="E7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F7" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="G7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -5628,51 +6661,51 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>624</v>
+        <v>599</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="B8" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C8" t="s">
-        <v>625</v>
+        <v>601</v>
       </c>
       <c r="D8" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -5684,51 +6717,51 @@
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>626</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="B9" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C9" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="D9" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -5740,51 +6773,51 @@
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>627</v>
+        <v>603</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>581</v>
+        <v>604</v>
       </c>
       <c r="B10" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C10" t="s">
-        <v>625</v>
+        <v>601</v>
       </c>
       <c r="D10" t="s">
-        <v>621</v>
+        <v>594</v>
       </c>
       <c r="E10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F10" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="G10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="K10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N10" t="s">
-        <v>628</v>
+        <v>605</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -5796,51 +6829,51 @@
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>629</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>581</v>
+        <v>604</v>
       </c>
       <c r="B11" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C11" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D11" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="K11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N11" t="s">
-        <v>630</v>
+        <v>607</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -5852,51 +6885,51 @@
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>631</v>
+        <v>608</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="B12" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C12" t="s">
-        <v>632</v>
+        <v>610</v>
       </c>
       <c r="D12" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -5908,51 +6941,51 @@
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>633</v>
+        <v>611</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="B13" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C13" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D13" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -5964,51 +6997,51 @@
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>634</v>
+        <v>612</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>585</v>
+        <v>613</v>
       </c>
       <c r="B14" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C14" t="s">
-        <v>632</v>
+        <v>610</v>
       </c>
       <c r="D14" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -6020,51 +7053,51 @@
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>635</v>
+        <v>614</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>585</v>
+        <v>613</v>
       </c>
       <c r="B15" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C15" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D15" t="s">
-        <v>621</v>
+        <v>594</v>
       </c>
       <c r="E15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F15" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="G15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -6076,51 +7109,51 @@
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>636</v>
+        <v>615</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B16" t="s">
-        <v>637</v>
+        <v>616</v>
       </c>
       <c r="C16" t="s">
-        <v>638</v>
+        <v>617</v>
       </c>
       <c r="D16" t="s">
-        <v>621</v>
+        <v>594</v>
       </c>
       <c r="E16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F16" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="G16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -6132,48 +7165,48 @@
         <v>1</v>
       </c>
       <c r="R16" t="s">
-        <v>639</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B17" t="s">
-        <v>614</v>
+        <v>587</v>
       </c>
       <c r="D17" t="s">
-        <v>615</v>
+        <v>588</v>
       </c>
       <c r="E17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N17" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -6185,51 +7218,51 @@
         <v>1</v>
       </c>
       <c r="R17" t="s">
-        <v>640</v>
+        <v>619</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
+        <v>595</v>
+      </c>
+      <c r="B18" t="s">
+        <v>542</v>
+      </c>
+      <c r="C18" t="s">
+        <v>549</v>
+      </c>
+      <c r="D18" t="s">
         <v>590</v>
       </c>
-      <c r="B18" t="s">
-        <v>541</v>
-      </c>
-      <c r="C18" t="s">
-        <v>548</v>
-      </c>
-      <c r="D18" t="s">
-        <v>617</v>
-      </c>
       <c r="E18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N18" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -6241,51 +7274,51 @@
         <v>1</v>
       </c>
       <c r="R18" t="s">
-        <v>641</v>
+        <v>620</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>588</v>
+        <v>621</v>
       </c>
       <c r="B19" t="s">
-        <v>637</v>
+        <v>616</v>
       </c>
       <c r="C19" t="s">
-        <v>638</v>
+        <v>617</v>
       </c>
       <c r="D19" t="s">
-        <v>621</v>
+        <v>594</v>
       </c>
       <c r="E19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F19" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="G19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="K19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N19" t="s">
-        <v>628</v>
+        <v>605</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -6297,51 +7330,51 @@
         <v>1</v>
       </c>
       <c r="R19" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>588</v>
+        <v>621</v>
       </c>
       <c r="B20" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C20" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D20" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="K20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N20" t="s">
-        <v>630</v>
+        <v>607</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -6353,48 +7386,48 @@
         <v>1</v>
       </c>
       <c r="R20" t="s">
-        <v>643</v>
+        <v>623</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="B21" t="s">
-        <v>614</v>
+        <v>587</v>
       </c>
       <c r="D21" t="s">
-        <v>615</v>
+        <v>588</v>
       </c>
       <c r="E21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N21" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O21">
         <v>1</v>
@@ -6406,51 +7439,51 @@
         <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>644</v>
+        <v>625</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="B22" t="s">
-        <v>645</v>
+        <v>626</v>
       </c>
       <c r="C22" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D22" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="E22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -6462,51 +7495,51 @@
         <v>1</v>
       </c>
       <c r="R22" t="s">
-        <v>647</v>
+        <v>628</v>
       </c>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="B23" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C23" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D23" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -6518,599 +7551,676 @@
         <v>1</v>
       </c>
       <c r="R23" t="s">
-        <v>648</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="15.8518518518519" customWidth="1"/>
+    <col min="3" max="3" width="14.4259259259259" customWidth="1"/>
+    <col min="4" max="4" width="13.1388888888889" customWidth="1"/>
+    <col min="5" max="5" width="9.71296296296296" customWidth="1"/>
+    <col min="6" max="6" width="19.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>676</v>
+        <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>667</v>
+        <v>631</v>
       </c>
       <c r="B2" t="s">
-        <v>574</v>
+        <v>632</v>
       </c>
       <c r="C2" t="s">
-        <v>668</v>
+        <v>633</v>
       </c>
       <c r="D2" t="s">
-        <v>669</v>
+        <v>634</v>
       </c>
       <c r="E2" t="s">
-        <v>564</v>
+        <v>635</v>
       </c>
       <c r="F2" t="s">
-        <v>613</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="B3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="C3" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="D3" t="s">
-        <v>670</v>
+        <v>636</v>
       </c>
       <c r="E3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F3" t="s">
-        <v>671</v>
+        <v>637</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="B4" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="C4" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="D4" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F4" t="s">
-        <v>672</v>
+        <v>638</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="B5" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="C5" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="D5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F5" t="s">
-        <v>673</v>
+        <v>639</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B6" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C6" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="D6" t="s">
-        <v>670</v>
+        <v>636</v>
       </c>
       <c r="E6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F6" t="s">
-        <v>674</v>
+        <v>640</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="B7" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="C7" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="D7" t="s">
-        <v>670</v>
+        <v>636</v>
       </c>
       <c r="E7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F7" t="s">
-        <v>675</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="109.222222222222" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>568</v>
+        <v>642</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B2" t="s">
-        <v>562</v>
+        <v>643</v>
       </c>
       <c r="C2" t="s">
-        <v>563</v>
+        <v>644</v>
       </c>
       <c r="D2" t="s">
-        <v>564</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B3" t="s">
-        <v>565</v>
+        <v>645</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B4" t="s">
-        <v>566</v>
+        <v>646</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B5" t="s">
-        <v>567</v>
+        <v>647</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="8.85185185185185" customWidth="1"/>
+    <col min="3" max="3" width="17.8518518518519" customWidth="1"/>
+    <col min="4" max="4" width="29.287037037037" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="7.42592592592593" customWidth="1"/>
+    <col min="7" max="7" width="15.8518518518519" customWidth="1"/>
+    <col min="8" max="8" width="19.4259259259259" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>594</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B2" t="s">
-        <v>569</v>
+        <v>649</v>
       </c>
       <c r="C2" t="s">
-        <v>570</v>
+        <v>650</v>
       </c>
       <c r="D2" t="s">
-        <v>571</v>
+        <v>651</v>
       </c>
       <c r="E2" t="s">
-        <v>572</v>
+        <v>652</v>
       </c>
       <c r="F2" t="s">
-        <v>573</v>
+        <v>653</v>
       </c>
       <c r="G2" t="s">
-        <v>574</v>
+        <v>632</v>
       </c>
       <c r="H2" t="s">
-        <v>575</v>
+        <v>654</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>576</v>
+        <v>597</v>
       </c>
       <c r="D3" t="s">
-        <v>577</v>
+        <v>655</v>
       </c>
       <c r="E3" t="s">
-        <v>578</v>
+        <v>656</v>
       </c>
       <c r="F3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="H3" t="s">
-        <v>580</v>
+        <v>657</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>581</v>
+        <v>604</v>
       </c>
       <c r="D4" t="s">
-        <v>582</v>
+        <v>658</v>
       </c>
       <c r="E4" t="s">
-        <v>578</v>
+        <v>656</v>
       </c>
       <c r="F4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G4" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="H4" t="s">
-        <v>584</v>
+        <v>659</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>585</v>
+        <v>613</v>
       </c>
       <c r="D5" t="s">
-        <v>586</v>
+        <v>660</v>
       </c>
       <c r="E5" t="s">
-        <v>578</v>
+        <v>656</v>
       </c>
       <c r="F5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G5" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="H5" t="s">
-        <v>584</v>
+        <v>659</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>588</v>
+        <v>621</v>
       </c>
       <c r="D6" t="s">
-        <v>589</v>
+        <v>661</v>
       </c>
       <c r="E6" t="s">
-        <v>578</v>
+        <v>656</v>
       </c>
       <c r="F6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G6" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="H6" t="s">
-        <v>580</v>
+        <v>657</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D7" t="s">
-        <v>591</v>
+        <v>662</v>
       </c>
       <c r="E7" t="s">
-        <v>578</v>
+        <v>656</v>
       </c>
       <c r="F7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G7" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="H7" t="s">
-        <v>593</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <cols>
+    <col min="5" max="5" width="41.1111111111111" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>596</v>
+        <v>568</v>
       </c>
       <c r="B2" t="s">
-        <v>574</v>
+        <v>632</v>
       </c>
       <c r="C2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D2" t="s">
-        <v>649</v>
+        <v>665</v>
       </c>
       <c r="E2" t="s">
-        <v>650</v>
+        <v>666</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="B3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="C3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D3" t="s">
-        <v>651</v>
+        <v>667</v>
       </c>
       <c r="E3" t="s">
-        <v>652</v>
+        <v>668</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>576</v>
+        <v>597</v>
       </c>
       <c r="B4" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="C4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D4" t="s">
-        <v>653</v>
+        <v>669</v>
       </c>
       <c r="E4" t="s">
-        <v>654</v>
+        <v>670</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="B5" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="C5" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D5" t="s">
-        <v>638</v>
+        <v>617</v>
       </c>
       <c r="E5" t="s">
-        <v>655</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>581</v>
+        <v>604</v>
       </c>
       <c r="B6" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="C6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D6" t="s">
-        <v>656</v>
+        <v>672</v>
       </c>
       <c r="E6" t="s">
-        <v>657</v>
+        <v>673</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="B7" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="C7" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D7" t="s">
-        <v>658</v>
+        <v>674</v>
       </c>
       <c r="E7" t="s">
-        <v>659</v>
+        <v>675</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>585</v>
+        <v>613</v>
       </c>
       <c r="B8" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="C8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D8" t="s">
-        <v>660</v>
+        <v>676</v>
       </c>
       <c r="E8" t="s">
-        <v>661</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B9" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C9" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D9" t="s">
-        <v>620</v>
+        <v>593</v>
       </c>
       <c r="E9" t="s">
-        <v>662</v>
+        <v>678</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>588</v>
+        <v>621</v>
       </c>
       <c r="B10" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D10" t="s">
-        <v>663</v>
+        <v>679</v>
       </c>
       <c r="E10" t="s">
-        <v>664</v>
+        <v>680</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="B11" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="D11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E11" t="s">
-        <v>665</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>688</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>